<commit_message>
update for the retrieve
</commit_message>
<xml_diff>
--- a/data/esg_retrieve/retrieve_questions.xlsx
+++ b/data/esg_retrieve/retrieve_questions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eddieho/Documents/NUS/DSS5105-PRJ/ESG/data/esg_retrieve/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FE9B25F3-293D-A14E-B34D-39F32BA00811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2AE308B-5A99-2A47-B071-6E12066E0EAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="340" yWindow="500" windowWidth="28100" windowHeight="16100" xr2:uid="{82FDEC40-F313-AD47-99D4-F2A47FA08EAF}"/>
+    <workbookView xWindow="6640" yWindow="1180" windowWidth="28100" windowHeight="16100" xr2:uid="{82FDEC40-F313-AD47-99D4-F2A47FA08EAF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
   <si>
     <t>What were the total greenhouse gas emissions (in tCO2e) for the reporting period?</t>
   </si>
@@ -305,6 +305,22 @@
   </si>
   <si>
     <t>What are all the relevant sustainability or ESG-related certifications held by the organization?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>What is the total number and rate of employee turnover during the reporting period?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>What is the total number of employees at the end of the reporting period?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B-SOC-EMP-TNM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B-SOC-EMP-TTN</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -701,10 +717,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF7C70D5-17CA-2441-BCC4-A37A8A077B87}">
-  <dimension ref="A1:B44"/>
+  <dimension ref="A1:B46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -947,121 +963,137 @@
     </row>
     <row r="30" spans="1:2" ht="18">
       <c r="A30" s="1" t="s">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>28</v>
+        <v>89</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="18">
       <c r="A31" s="1" t="s">
-        <v>68</v>
+        <v>91</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>29</v>
+        <v>88</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="18">
       <c r="A32" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="18">
       <c r="A33" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="18">
       <c r="A34" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="18">
       <c r="A35" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="18">
       <c r="A36" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="18">
       <c r="A37" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="18">
       <c r="A38" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="18">
       <c r="A39" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>84</v>
+        <v>35</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="18">
       <c r="A40" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="18">
       <c r="A41" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="19">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="18">
       <c r="A42" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>87</v>
+        <v>77</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="18">
       <c r="A43" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="19">
+      <c r="A44" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="18">
+      <c r="A45" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B45" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="18">
-      <c r="A44" s="1" t="s">
+    <row r="46" spans="1:2" ht="18">
+      <c r="A46" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B46" s="1" t="s">
         <v>86</v>
       </c>
     </row>

</xml_diff>

<commit_message>
edit label and clean data output file
</commit_message>
<xml_diff>
--- a/data/esg_retrieve/retrieve_questions.xlsx
+++ b/data/esg_retrieve/retrieve_questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eddieho/Documents/NUS/DSS5105-PRJ/ESG/data/esg_retrieve/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{166F750C-2106-A548-AEA1-19605A73E2EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B5F461F-CB40-8C43-B6B4-CC9F62968086}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="700" yWindow="500" windowWidth="28100" windowHeight="16100" xr2:uid="{82FDEC40-F313-AD47-99D4-F2A47FA08EAF}"/>
   </bookViews>
@@ -312,15 +312,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>B-SOC-EMP-TNM</t>
+    <t>What is the total number of employee turnover during the reporting period?</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>B-SOC-EMP-TTN</t>
+    <t>B-SOC_EMP_TNM</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>What is the total number of employee turnover during the reporting period?</t>
+    <t>B-SOC_EMP_TTN</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -719,8 +719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF7C70D5-17CA-2441-BCC4-A37A8A077B87}">
   <dimension ref="A1:B46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B18" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -963,7 +963,7 @@
     </row>
     <row r="30" spans="1:2" ht="18">
       <c r="A30" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>88</v>
@@ -971,10 +971,10 @@
     </row>
     <row r="31" spans="1:2" ht="18">
       <c r="A31" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="18">

</xml_diff>